<commit_message>
Add option to provide files locally and skip downloading the FASTQs
</commit_message>
<xml_diff>
--- a/examples/processing_metadata_template.xlsx
+++ b/examples/processing_metadata_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Sequencing core project</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>XXXXXXX</t>
+  </si>
+  <si>
+    <t>with ercc spike-in</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -822,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,7 +856,7 @@
     <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -884,8 +890,11 @@
       <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -940,7 +949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -968,8 +977,11 @@
       <c r="J4" t="s">
         <v>15</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -997,8 +1009,11 @@
       <c r="J5" t="s">
         <v>15</v>
       </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1027,7 +1042,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Add STARR-seq notebook generation logic
</commit_message>
<xml_diff>
--- a/examples/processing_metadata_template.xlsx
+++ b/examples/processing_metadata_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>Sequencing core project</t>
   </si>
@@ -138,13 +138,22 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>STARR-seq</t>
+  </si>
+  <si>
+    <t>CAL51.starrseq.Gefit.rep1</t>
+  </si>
+  <si>
+    <t>CAL51.starrseq.Gefit_Inibit.rep1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,6 +183,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -192,7 +208,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="148">
+  <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,12 +357,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="148">
+  <cellStyles count="150">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -422,6 +441,7 @@
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -494,6 +514,7 @@
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -828,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,6 +1092,66 @@
         <v>32</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add STARR-seq with UMIs notebook generation logic
</commit_message>
<xml_diff>
--- a/examples/processing_metadata_template.xlsx
+++ b/examples/processing_metadata_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26920" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="14640" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
   <si>
     <t>Sequencing core project</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>CAL51.starrseq.Gefit_Inibit.rep1</t>
+  </si>
+  <si>
+    <t>UMIs</t>
   </si>
 </sst>
 </file>
@@ -849,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,19 +868,20 @@
     <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -903,19 +907,22 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -941,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -966,11 +973,11 @@
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -995,14 +1002,14 @@
       <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1027,14 +1034,14 @@
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1059,11 +1066,11 @@
       <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1088,11 +1095,11 @@
       <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1117,12 +1124,15 @@
       <c r="H8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1147,10 +1157,13 @@
       <c r="H9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>